<commit_message>
it's related to moustache jsonType template with .moustache file
</commit_message>
<xml_diff>
--- a/PythonBasic/PythonInit/resources/test-data.xlsx
+++ b/PythonBasic/PythonInit/resources/test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\My Drive\Vivid-Vortex-git-repo\Python\PythonBasic\PythonInit\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739F49E6-3B20-49CD-813F-8CA819EF0F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A560780E-5BD1-43D0-A470-6E11A51BE2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="req-payload" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>follower</t>
+  </si>
+  <si>
+    <t>address.city</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Bombay</t>
   </si>
 </sst>
 </file>
@@ -376,15 +385,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E2075C-906D-443E-BEC2-D1D483787489}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +408,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -405,15 +422,26 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -426,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071D3BED-DBF0-49E3-AFDB-A85D198028AD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
list of uniquw dictionary
</commit_message>
<xml_diff>
--- a/PythonBasic/PythonInit/resources/test-data.xlsx
+++ b/PythonBasic/PythonInit/resources/test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\My Drive\Vivid-Vortex-git-repo\Python\PythonBasic\PythonInit\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A560780E-5BD1-43D0-A470-6E11A51BE2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4126F504-8335-467A-B967-B91FCD8D9C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>Bombay</t>
+  </si>
+  <si>
+    <t>address.lane</t>
+  </si>
+  <si>
+    <t>lane 1</t>
+  </si>
+  <si>
+    <t>lane 2</t>
+  </si>
+  <si>
+    <t>contact.phone</t>
+  </si>
+  <si>
+    <t>contact.email</t>
+  </si>
+  <si>
+    <t>deepak.kumar@gmail.com</t>
+  </si>
+  <si>
+    <t>kumar.deepak@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -385,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E2075C-906D-443E-BEC2-D1D483787489}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,9 +417,12 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +435,17 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,16 +458,34 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>9206918946</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>9206918947</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>

</xml_diff>